<commit_message>
revised the welfare indicator to average hh weekly expenditure
</commit_message>
<xml_diff>
--- a/baseline/baseline_indicators/MI_WP3_Ug_maize_baseline_Indicators.xlsx
+++ b/baseline/baseline_indicators/MI_WP3_Ug_maize_baseline_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/baseline/baseline_indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC812796-BDB5-4799-8D4F-27B88FEAEF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{CC812796-BDB5-4799-8D4F-27B88FEAEF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8C92122-FA26-4D01-AAB1-CA93DE22C54A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="668" xr2:uid="{538A9C85-F0F7-4C66-A0DE-0201E7D515F7}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="158">
   <si>
     <t>Indicator</t>
   </si>
@@ -115,9 +115,6 @@
     <t>USD</t>
   </si>
   <si>
-    <t>Include exchange rate used (or other welfare indicator used if income not available)</t>
-  </si>
-  <si>
     <t>km</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t>Value of (standard/past) harvest</t>
-  </si>
-  <si>
-    <t>Explain if alternate indicator was used</t>
   </si>
   <si>
     <t>% of Harvest Value Consumed by HH</t>
@@ -319,25 +313,6 @@
     </r>
   </si>
   <si>
-    <t># of rooms</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Distance to Nearest Market (/other remoteness measure)- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to agro-inpu shop selling maize seed</t>
-    </r>
-  </si>
-  <si>
     <t>N (pooled sample)</t>
   </si>
   <si>
@@ -899,6 +874,36 @@
     </r>
   </si>
   <si>
+    <t>A-WEAI Score- Unable to calculate this due to data gaps. However, refer to sheet 5 for some women indicators</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Uganda Maize</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster random sampling was employed. Using a sampling frame from the Uganda National Bureau of Statistics, villages (the clusters) in the study districts were randomly selected, with probability proportionate to the number of households living in the village. </t>
+  </si>
+  <si>
+    <t>Yes, we can use variation in the household head's gender. During samping, we used the village households lists kept by the village leaders to randomly select every (N/10)th household on the list, and this ensured that every male or female headed household had the same chance of being selected.</t>
+  </si>
+  <si>
+    <t>These are Kenyan. The NARO scientist indicated that they have no means of tracking them</t>
+  </si>
+  <si>
+    <t>The year of release is not available on the NARO list of varieties. So the years were estimated based on the highest number of years that farmers reported to have been using landraces.</t>
+  </si>
+  <si>
+    <t>Variety grown in the second season of 2022</t>
+  </si>
+  <si>
+    <t>Source of info/comment for the year of release</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Average Income (/other welfare indicator--- </t>
     </r>
@@ -911,7 +916,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Percapita living space (percapita rooms in the household</t>
+      <t>Average household weekly expenditure</t>
     </r>
     <r>
       <rPr>
@@ -925,34 +930,44 @@
     </r>
   </si>
   <si>
-    <t>A-WEAI Score- Unable to calculate this due to data gaps. However, refer to sheet 5 for some women indicators</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Uganda Maize</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluster random sampling was employed. Using a sampling frame from the Uganda National Bureau of Statistics, villages (the clusters) in the study districts were randomly selected, with probability proportionate to the number of households living in the village. </t>
-  </si>
-  <si>
-    <t>Yes, we can use variation in the household head's gender. During samping, we used the village households lists kept by the village leaders to randomly select every (N/10)th household on the list, and this ensured that every male or female headed household had the same chance of being selected.</t>
-  </si>
-  <si>
-    <t>These are Kenyan. The NARO scientist indicated that they have no means of tracking them</t>
-  </si>
-  <si>
-    <t>The year of release is not available on the NARO list of varieties. So the years were estimated based on the highest number of years that farmers reported to have been using landraces.</t>
-  </si>
-  <si>
-    <t>Variety grown in the second season of 2022</t>
-  </si>
-  <si>
-    <t>Source of info/comment for the year of release</t>
+    <r>
+      <t>Distance to Nearest Market (/other remoteness measure)/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to nearest agro-inpu shop selling maize seed</t>
+    </r>
+  </si>
+  <si>
+    <t>1USD = 3720.75 Ug shillings. The welfare indicator used is the household weekly expenditure on food (includng fruits, vegetables) salt, soap, cooking oil, and airtime).</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1588,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1593,7 +1608,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1609,10 +1624,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1620,32 +1635,32 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1666,12 +1681,12 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q15" sqref="Q15"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
@@ -1695,7 +1710,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1722,27 +1737,27 @@
         <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="29">
         <v>2319</v>
@@ -1781,7 +1796,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="29">
         <v>2319</v>
@@ -1828,7 +1843,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="29">
         <v>2319</v>
@@ -1872,7 +1887,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1919,7 +1934,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1966,7 +1981,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -2013,7 +2028,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -2060,10 +2075,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="29">
         <v>1598</v>
@@ -2107,10 +2122,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="29">
         <v>2319</v>
@@ -2204,107 +2219,105 @@
         <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N12" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O12" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="P12" s="39" t="s">
-        <v>24</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="P12" s="39"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>149</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>80</v>
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="29">
         <v>2319</v>
       </c>
       <c r="D13" s="25">
-        <v>0.49299999999999999</v>
+        <v>3.819</v>
       </c>
       <c r="E13" s="25">
-        <v>0.32500000000000001</v>
+        <v>2.4319999999999999</v>
       </c>
       <c r="F13" s="25">
-        <v>0.47299999999999998</v>
+        <v>3.6739999999999999</v>
       </c>
       <c r="G13" s="25">
-        <v>0.26700000000000002</v>
+        <v>2.093</v>
       </c>
       <c r="H13" s="25">
-        <v>0.505</v>
+        <v>3.847</v>
       </c>
       <c r="I13" s="25">
-        <v>0.34499999999999997</v>
+        <v>2.5619999999999998</v>
       </c>
       <c r="J13" s="25">
-        <v>0.48099999999999998</v>
+        <v>3.7480000000000002</v>
       </c>
       <c r="K13" s="25">
-        <v>0.32500000000000001</v>
+        <v>2.109</v>
       </c>
       <c r="L13" s="25">
-        <v>0.47199999999999998</v>
+        <v>3.871</v>
       </c>
       <c r="M13" s="25">
-        <v>0.30399999999999999</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="N13" s="25">
-        <v>0.57499999999999996</v>
+        <v>3.6190000000000002</v>
       </c>
       <c r="O13" s="25">
-        <v>0.38400000000000001</v>
+        <v>1.92</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="29">
         <v>2200</v>
@@ -2348,19 +2361,19 @@
     </row>
     <row r="15" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F15" s="40"/>
       <c r="G15" s="40"/>
@@ -2369,24 +2382,24 @@
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
       <c r="L15" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M15" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N15" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O15" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="29">
         <v>2319</v>
@@ -2418,10 +2431,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="29">
         <v>2319</v>
@@ -2453,10 +2466,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
         <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
       </c>
       <c r="C18" s="29">
         <v>2319</v>
@@ -2468,22 +2481,22 @@
         <v>0.47299999999999998</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L18">
         <v>0.33</v>
@@ -2500,10 +2513,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="29">
         <v>2319</v>
@@ -2515,22 +2528,22 @@
         <v>0.37</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L19">
         <v>0.16900000000000001</v>
@@ -2547,10 +2560,10 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="29">
         <v>2319</v>
@@ -2562,22 +2575,22 @@
         <v>0.37</v>
       </c>
       <c r="F20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L20">
         <v>0.154</v>
@@ -2605,7 +2618,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2633,7 +2646,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -2660,27 +2673,27 @@
         <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="29">
         <v>2311</v>
@@ -2724,10 +2737,10 @@
     </row>
     <row r="3" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="29">
         <v>2318</v>
@@ -2771,7 +2784,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -2816,12 +2829,12 @@
         <v>99.789000000000001</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2868,7 +2881,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -2915,57 +2928,57 @@
     </row>
     <row r="7" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O7" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="29">
         <v>2306</v>
@@ -3009,10 +3022,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="29">
         <v>927</v>
@@ -3056,10 +3069,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C10" s="29">
         <v>1428</v>
@@ -3103,10 +3116,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="29">
         <v>2238</v>
@@ -3150,10 +3163,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="29">
         <v>2238</v>
@@ -3197,10 +3210,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="29">
         <v>2238</v>
@@ -3244,7 +3257,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -3291,7 +3304,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -3338,57 +3351,57 @@
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O16" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" t="s">
         <v>103</v>
-      </c>
-      <c r="B17" t="s">
-        <v>107</v>
       </c>
       <c r="C17" s="29">
         <v>2317</v>
@@ -3430,15 +3443,15 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="P17" s="34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C18" s="29">
         <v>2302</v>
@@ -3483,10 +3496,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C19" s="29">
         <v>2306</v>
@@ -3531,10 +3544,10 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C20" s="29">
         <v>2311</v>
@@ -3576,102 +3589,102 @@
         <v>0.79100000000000004</v>
       </c>
       <c r="P20" s="35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O21" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P21" s="38"/>
     </row>
     <row r="22" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O22" s="37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P22" s="38"/>
     </row>
@@ -3750,19 +3763,19 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
@@ -3771,7 +3784,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -3786,13 +3799,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -3812,10 +3825,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="4" t="s">
@@ -3833,7 +3846,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="4" t="s">
@@ -3851,7 +3864,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="4" t="s">
@@ -3869,7 +3882,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="4" t="s">
@@ -3888,7 +3901,7 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="6" t="s">
@@ -3911,10 +3924,10 @@
     </row>
     <row r="8" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="30" t="s">
@@ -3925,7 +3938,7 @@
     <row r="9" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32"/>
       <c r="B9" s="30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="30" t="s">
@@ -3936,7 +3949,7 @@
     <row r="10" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32"/>
       <c r="B10" s="30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="30" t="s">
@@ -3947,7 +3960,7 @@
     <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="33"/>
       <c r="B11" s="31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="31" t="s">
@@ -3964,10 +3977,10 @@
     </row>
     <row r="12" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="30" t="s">
@@ -3978,7 +3991,7 @@
     <row r="13" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="32"/>
       <c r="B13" s="30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="30" t="s">
@@ -3988,7 +4001,7 @@
     </row>
     <row r="14" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="30" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="30" t="s">
@@ -3999,7 +4012,7 @@
     <row r="15" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="31" t="s">
@@ -4016,10 +4029,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="4" t="s">
@@ -4037,7 +4050,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="4" t="s">
@@ -4055,7 +4068,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="4" t="s">
@@ -4073,7 +4086,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="4" t="s">
@@ -4092,7 +4105,7 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="6" t="s">
@@ -4115,10 +4128,10 @@
     </row>
     <row r="21" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -4133,21 +4146,21 @@
     </row>
     <row r="22" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="41" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="41"/>
       <c r="B23" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
@@ -4162,17 +4175,17 @@
     </row>
     <row r="24" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
@@ -4188,11 +4201,11 @@
     <row r="26" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19"/>
       <c r="B26" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="19"/>
@@ -4254,7 +4267,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -4281,27 +4294,27 @@
         <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="29">
         <v>2319</v>
@@ -4345,10 +4358,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="29">
         <v>2319</v>
@@ -4393,10 +4406,10 @@
     </row>
     <row r="4" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="29">
         <v>590</v>
@@ -4440,10 +4453,10 @@
     </row>
     <row r="5" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="29">
         <v>646</v>
@@ -4487,10 +4500,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="29">
         <v>2319</v>
@@ -4534,10 +4547,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="29">
         <v>2319</v>
@@ -4581,7 +4594,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -4628,7 +4641,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -4675,7 +4688,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -4722,7 +4735,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -4769,7 +4782,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -4816,7 +4829,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -4863,7 +4876,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -4910,7 +4923,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -4957,7 +4970,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C16" s="29">
         <v>959</v>
@@ -5117,7 +5130,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5129,29 +5142,29 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" s="32">
         <v>2009</v>
@@ -5160,121 +5173,121 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B4" s="32">
         <v>2000</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B5" s="32">
         <v>2013</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C6" s="32"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B7" s="32">
         <v>2000</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B8" s="32">
         <v>2003</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B9" s="32">
         <v>2002</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B10" s="32">
         <v>2002</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B12" s="32">
         <v>2002</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B13" s="32">
         <v>2016</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B14">
         <v>2014</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>